<commit_message>
Added changes for Easy solution maths , array and Strings
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82485948fb58841c/Desktop/leetcode/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0B821F-750C-4990-B279-49DFBFD5993A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{7B0B821F-750C-4990-B279-49DFBFD5993A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC407905-9698-4CC0-9EAA-A5C29157DE6B}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="388">
   <si>
     <r>
       <rPr>
@@ -1719,8 +1719,8 @@
   </sheetPr>
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="A140" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1730,7 +1730,7 @@
     <col min="3" max="3" width="62.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1741,22 +1741,22 @@
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>6</v>
       </c>
@@ -2055,32 +2055,32 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B49" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B51" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B52" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B53" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B54" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B55" s="7" t="s">
         <v>71</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="56" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B56" s="7" t="s">
         <v>73</v>
       </c>
@@ -2096,27 +2096,33 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B58" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="59" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B59" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>387</v>
+      </c>
       <c r="B60" s="6" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>387</v>
+      </c>
       <c r="B61" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B62" s="7" t="s">
         <v>78</v>
       </c>
@@ -2124,7 +2130,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="63" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B63" s="6" t="s">
         <v>80</v>
       </c>
@@ -2296,67 +2302,82 @@
         <v>113</v>
       </c>
     </row>
-    <row r="97" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="98" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B98" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="100" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B100" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="101" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B101" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>387</v>
+      </c>
       <c r="B102" s="7" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="103" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>387</v>
+      </c>
       <c r="B103" s="7" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="104" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>387</v>
+      </c>
       <c r="B104" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="105" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>387</v>
+      </c>
       <c r="B105" s="7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="106" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>387</v>
+      </c>
       <c r="B106" s="7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="108" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B108" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="109" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B109" s="7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="110" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B110" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="111" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B111" s="7" t="s">
         <v>124</v>
       </c>
@@ -2439,37 +2460,52 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B130" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="131" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B131" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="132" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>387</v>
+      </c>
       <c r="B132" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="133" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>387</v>
+      </c>
       <c r="B133" s="7" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="134" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>387</v>
+      </c>
       <c r="B134" s="6" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="135" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>387</v>
+      </c>
       <c r="B135" s="6" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="136" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>387</v>
+      </c>
       <c r="B136" s="6" t="s">
         <v>145</v>
       </c>
@@ -2477,37 +2513,49 @@
         <v>146</v>
       </c>
     </row>
-    <row r="137" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>387</v>
+      </c>
       <c r="B137" s="6" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="138" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>387</v>
+      </c>
       <c r="B138" s="6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="139" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>387</v>
+      </c>
       <c r="B139" s="6" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="140" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>387</v>
+      </c>
       <c r="B140" s="6" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="142" spans="2:3" ht="13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" ht="13" x14ac:dyDescent="0.3">
       <c r="B142" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="143" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B143" s="6" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="144" spans="2:3" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B144" s="6" t="s">
         <v>152</v>
       </c>

</xml_diff>

<commit_message>
Changes for Linked List
</commit_message>
<xml_diff>
--- a/Leetcode.xlsx
+++ b/Leetcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82485948fb58841c/Desktop/leetcode/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{7B0B821F-750C-4990-B279-49DFBFD5993A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B3E27CB-CA64-42FE-9D1F-033C467FA787}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{7B0B821F-750C-4990-B279-49DFBFD5993A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E39CD02B-B61C-4E9A-A5DD-0AF4C6A5C99D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="388">
   <si>
     <r>
       <rPr>
@@ -1728,8 +1728,8 @@
   </sheetPr>
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
-      <selection activeCell="A204" sqref="A204"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="A378" sqref="A378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3586,77 +3586,95 @@
         <v>332</v>
       </c>
     </row>
-    <row r="369" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B369" s="4" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="370" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B370" s="12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="371" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>387</v>
+      </c>
       <c r="B371" s="13" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="372" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>387</v>
+      </c>
       <c r="B372" s="14" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="373" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>387</v>
+      </c>
       <c r="B373" s="6" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="374" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>387</v>
+      </c>
       <c r="B374" s="6" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="375" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B375" s="6" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="376" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>387</v>
+      </c>
       <c r="B376" s="6" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="377" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>387</v>
+      </c>
       <c r="B377" s="6" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="378" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B378" s="6" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="379" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B379" s="6" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="380" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B380" s="6" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="381" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B381" s="6" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="382" spans="2:2" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:2" ht="12.5" x14ac:dyDescent="0.25">
       <c r="B382" s="6" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="384" spans="2:2" ht="13" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:2" ht="13" x14ac:dyDescent="0.3">
       <c r="B384" s="5" t="s">
         <v>31</v>
       </c>

</xml_diff>